<commit_message>
added data for part 2
</commit_message>
<xml_diff>
--- a/Lab2/Lab2_Data.xlsx
+++ b/Lab2/Lab2_Data.xlsx
@@ -8,19 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fliang/Labs/ECE358/Lab2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8815B93B-5155-7945-935D-64A1663166E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CE61FC-787A-5B4F-9DBE-C84D9C278499}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10060" yWindow="460" windowWidth="18740" windowHeight="15940" xr2:uid="{CD3D1FDA-1D36-744E-9399-F59D5B515E4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$4:$A$8</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$4:$B$8</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$4:$C$8</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$4:$D$8</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -602,6 +596,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.18065899999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1585009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1266,6 +1263,9 @@
                 <c:pt idx="3">
                   <c:v>0.903443</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.91086800000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1829,6 +1829,21 @@
               <c:numCache>
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.999699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99920100000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99815399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99672700000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99470000000000003</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1899,6 +1914,21 @@
               <c:numCache>
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.99961500000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99809899999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.996147</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99322310000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98915900000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2033,7 +2063,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0"/>
+          <c:min val="0.98"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2467,6 +2497,21 @@
               <c:numCache>
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.29943900000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.60040099999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90180199999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.198401</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.4999089999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2537,6 +2582,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.59956699999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1986129999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.801671</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.398466</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0038809999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5501,8 +5561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8782A8-5F07-BD40-AC8C-8932D019AA2B}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5664,14 +5724,18 @@
       <c r="C8" s="18">
         <v>0.1585568</v>
       </c>
-      <c r="D8" s="18"/>
+      <c r="D8" s="18">
+        <v>0.1585009</v>
+      </c>
       <c r="E8" s="9">
         <v>0.88769500000000001</v>
       </c>
       <c r="F8" s="5">
         <v>0.91107899999999997</v>
       </c>
-      <c r="G8" s="6"/>
+      <c r="G8" s="6">
+        <v>0.91086800000000001</v>
+      </c>
       <c r="J8" s="17"/>
     </row>
     <row r="34" spans="1:7" ht="30" thickBot="1">
@@ -5722,13 +5786,21 @@
       <c r="B37" s="13">
         <v>0.99992899999999996</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
+      <c r="C37" s="16">
+        <v>0.999699</v>
+      </c>
+      <c r="D37" s="16">
+        <v>0.99961500000000003</v>
+      </c>
       <c r="E37" s="13">
         <v>0.210309</v>
       </c>
-      <c r="F37" s="16"/>
-      <c r="G37" s="14"/>
+      <c r="F37" s="16">
+        <v>0.29943900000000001</v>
+      </c>
+      <c r="G37" s="14">
+        <v>0.59956699999999996</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="21">
       <c r="A38" s="10">
@@ -5737,13 +5809,21 @@
       <c r="B38" s="8">
         <v>0.99944299999999997</v>
       </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
+      <c r="C38" s="15">
+        <v>0.99920100000000001</v>
+      </c>
+      <c r="D38" s="15">
+        <v>0.99809899999999996</v>
+      </c>
       <c r="E38" s="8">
         <v>0.420018</v>
       </c>
-      <c r="F38" s="15"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="15">
+        <v>0.60040099999999996</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1.1986129999999999</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="21">
       <c r="A39" s="10">
@@ -5752,13 +5832,21 @@
       <c r="B39" s="8">
         <v>0.99872700000000003</v>
       </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
+      <c r="C39" s="15">
+        <v>0.99815399999999999</v>
+      </c>
+      <c r="D39" s="15">
+        <v>0.996147</v>
+      </c>
       <c r="E39" s="8">
         <v>0.63061500000000004</v>
       </c>
-      <c r="F39" s="15"/>
-      <c r="G39" s="3"/>
+      <c r="F39" s="15">
+        <v>0.90180199999999999</v>
+      </c>
+      <c r="G39" s="3">
+        <v>1.801671</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="21">
       <c r="A40" s="10">
@@ -5767,13 +5855,21 @@
       <c r="B40" s="8">
         <v>0.99747699999999995</v>
       </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
+      <c r="C40" s="15">
+        <v>0.99672700000000003</v>
+      </c>
+      <c r="D40" s="15">
+        <v>0.99322310000000003</v>
+      </c>
       <c r="E40" s="8">
         <v>0.84013499999999997</v>
       </c>
-      <c r="F40" s="15"/>
-      <c r="G40" s="3"/>
+      <c r="F40" s="15">
+        <v>1.198401</v>
+      </c>
+      <c r="G40" s="3">
+        <v>2.398466</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="22" thickBot="1">
       <c r="A41" s="4">
@@ -5782,13 +5878,21 @@
       <c r="B41" s="9">
         <v>0.99615200000000004</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
+      <c r="C41" s="18">
+        <v>0.99470000000000003</v>
+      </c>
+      <c r="D41" s="18">
+        <v>0.98915900000000001</v>
+      </c>
       <c r="E41" s="9">
         <v>1.050063</v>
       </c>
-      <c r="F41" s="5"/>
-      <c r="G41" s="6"/>
+      <c r="F41" s="5">
+        <v>1.4999089999999999</v>
+      </c>
+      <c r="G41" s="6">
+        <v>3.0038809999999998</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
updated report and source code
</commit_message>
<xml_diff>
--- a/Lab2/Lab2_Data.xlsx
+++ b/Lab2/Lab2_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fliang/Labs/ECE358/Lab2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4320A7AD-A825-F743-AC58-A7EED0F90CE5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601E69C2-A634-804A-A195-B636EA4CD8EE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CD3D1FDA-1D36-744E-9399-F59D5B515E4C}"/>
   </bookViews>
@@ -217,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,14 +252,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1747,19 +1748,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.99975800000000004</c:v>
+                  <c:v>0.99979300000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99870899999999996</c:v>
+                  <c:v>0.99801600000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99637900000000001</c:v>
+                  <c:v>0.98100299999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99230399999999996</c:v>
+                  <c:v>0.92470699999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98779899999999998</c:v>
+                  <c:v>0.851464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1832,19 +1833,19 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.99965000000000004</c:v>
+                  <c:v>0.99963999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99770000000000003</c:v>
+                  <c:v>0.98659200000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99403799999999998</c:v>
+                  <c:v>0.90898500000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98631400000000002</c:v>
+                  <c:v>0.84872999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98825499999999999</c:v>
+                  <c:v>0.81433299999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1917,19 +1918,19 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.99902000000000002</c:v>
+                  <c:v>0.98799199999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99745700000000004</c:v>
+                  <c:v>0.92538600000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98608669999999998</c:v>
+                  <c:v>0.88785499999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98931500000000006</c:v>
+                  <c:v>0.84886899999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98313200000000001</c:v>
+                  <c:v>0.81329700000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2065,7 +2066,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.98"/>
+          <c:min val="0.70000000000000007"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2412,22 +2413,22 @@
             <c:numRef>
               <c:f>Sheet1!$E$37:$E$41</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.210428</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.20980799999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42010199999999998</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0.000000">
-                  <c:v>0.61995</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.78140699999999996</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.90247200000000005</c:v>
+                  <c:v>0.41944999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62005100000000002</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>0.78093299999999999</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>0.90350299999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2500,19 +2501,19 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.29978300000000002</c:v>
+                  <c:v>0.30007800000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.59209800000000001</c:v>
+                  <c:v>0.59390600000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.82397399999999998</c:v>
+                  <c:v>0.82318400000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.92222099999999996</c:v>
+                  <c:v>0.92223750000000004</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>0.96449300000000004</c:v>
+                  <c:v>0.96533899999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2585,19 +2586,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.59347499999999997</c:v>
+                  <c:v>0.593642</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.81442499999999995</c:v>
+                  <c:v>0.81279100000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.87388500000000002</c:v>
+                  <c:v>0.87451599999999996</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.000000">
-                  <c:v>0.92217000000000005</c:v>
+                  <c:v>0.92112899999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.962565</c:v>
+                  <c:v>0.96559499999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5563,8 +5564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8782A8-5F07-BD40-AC8C-8932D019AA2B}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5576,6 +5577,7 @@
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="37" customHeight="1" thickBot="1">
@@ -5584,7 +5586,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="21">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -5599,7 +5601,7 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="22" thickBot="1">
-      <c r="A3" s="21"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
@@ -5740,13 +5742,13 @@
       </c>
       <c r="J8" s="17"/>
     </row>
-    <row r="34" spans="1:7" ht="30" thickBot="1">
+    <row r="34" spans="1:9" ht="30" thickBot="1">
       <c r="A34" s="19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="21">
-      <c r="A35" s="20" t="s">
+    <row r="35" spans="1:9" ht="21">
+      <c r="A35" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="7" t="s">
@@ -5760,8 +5762,8 @@
       <c r="F35" s="1"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" ht="22" thickBot="1">
-      <c r="A36" s="21"/>
+    <row r="36" spans="1:9" ht="22" thickBot="1">
+      <c r="A36" s="23"/>
       <c r="B36" s="10" t="s">
         <v>3</v>
       </c>
@@ -5781,119 +5783,123 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="21">
+    <row r="37" spans="1:9" ht="21">
       <c r="A37" s="10">
         <v>20</v>
       </c>
       <c r="B37" s="13">
-        <v>0.99975800000000004</v>
+        <v>0.99979300000000004</v>
       </c>
       <c r="C37" s="16">
-        <v>0.99965000000000004</v>
+        <v>0.99963999999999997</v>
       </c>
       <c r="D37" s="16">
-        <v>0.99902000000000002</v>
+        <v>0.98799199999999998</v>
       </c>
       <c r="E37" s="13">
-        <v>0.210428</v>
+        <v>0.20980799999999999</v>
       </c>
       <c r="F37" s="16">
-        <v>0.29978300000000002</v>
+        <v>0.30007800000000001</v>
       </c>
       <c r="G37" s="14">
-        <v>0.59347499999999997</v>
-      </c>
+        <v>0.593642</v>
+      </c>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
     </row>
-    <row r="38" spans="1:7" ht="21">
+    <row r="38" spans="1:9" ht="21">
       <c r="A38" s="10">
         <v>40</v>
       </c>
       <c r="B38" s="8">
-        <v>0.99870899999999996</v>
+        <v>0.99801600000000001</v>
       </c>
       <c r="C38" s="15">
-        <v>0.99770000000000003</v>
+        <v>0.98659200000000002</v>
       </c>
       <c r="D38" s="15">
-        <v>0.99745700000000004</v>
-      </c>
-      <c r="E38" s="8">
-        <v>0.42010199999999998</v>
+        <v>0.92538600000000004</v>
+      </c>
+      <c r="E38" s="21">
+        <v>0.41944999999999999</v>
       </c>
       <c r="F38" s="15">
-        <v>0.59209800000000001</v>
+        <v>0.59390600000000004</v>
       </c>
       <c r="G38" s="3">
-        <v>0.81442499999999995</v>
-      </c>
+        <v>0.81279100000000004</v>
+      </c>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
     </row>
-    <row r="39" spans="1:7" ht="21">
+    <row r="39" spans="1:9" ht="21">
       <c r="A39" s="10">
         <v>60</v>
       </c>
       <c r="B39" s="8">
-        <v>0.99637900000000001</v>
+        <v>0.98100299999999996</v>
       </c>
       <c r="C39" s="15">
-        <v>0.99403799999999998</v>
+        <v>0.90898500000000004</v>
       </c>
       <c r="D39" s="15">
-        <v>0.98608669999999998</v>
-      </c>
-      <c r="E39" s="23">
-        <v>0.61995</v>
+        <v>0.88785499999999995</v>
+      </c>
+      <c r="E39" s="21">
+        <v>0.62005100000000002</v>
       </c>
       <c r="F39" s="15">
-        <v>0.82397399999999998</v>
+        <v>0.82318400000000003</v>
       </c>
       <c r="G39" s="3">
-        <v>0.87388500000000002</v>
+        <v>0.87451599999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="21">
+    <row r="40" spans="1:9" ht="21">
       <c r="A40" s="10">
         <v>80</v>
       </c>
       <c r="B40" s="8">
-        <v>0.99230399999999996</v>
+        <v>0.92470699999999995</v>
       </c>
       <c r="C40" s="15">
-        <v>0.98631400000000002</v>
+        <v>0.84872999999999998</v>
       </c>
       <c r="D40" s="15">
-        <v>0.98931500000000006</v>
+        <v>0.84886899999999998</v>
       </c>
       <c r="E40" s="8">
-        <v>0.78140699999999996</v>
+        <v>0.78093299999999999</v>
       </c>
       <c r="F40" s="15">
-        <v>0.92222099999999996</v>
-      </c>
-      <c r="G40" s="22">
-        <v>0.92217000000000005</v>
+        <v>0.92223750000000004</v>
+      </c>
+      <c r="G40" s="20">
+        <v>0.92112899999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="22" thickBot="1">
+    <row r="41" spans="1:9" ht="22" thickBot="1">
       <c r="A41" s="4">
         <v>100</v>
       </c>
       <c r="B41" s="9">
-        <v>0.98779899999999998</v>
+        <v>0.851464</v>
       </c>
       <c r="C41" s="18">
-        <v>0.98825499999999999</v>
+        <v>0.81433299999999997</v>
       </c>
       <c r="D41" s="18">
-        <v>0.98313200000000001</v>
+        <v>0.81329700000000005</v>
       </c>
       <c r="E41" s="9">
-        <v>0.90247200000000005</v>
+        <v>0.90350299999999995</v>
       </c>
       <c r="F41" s="5">
-        <v>0.96449300000000004</v>
+        <v>0.96533899999999995</v>
       </c>
       <c r="G41" s="6">
-        <v>0.962565</v>
+        <v>0.96559499999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>